<commit_message>
all our tests passing
</commit_message>
<xml_diff>
--- a/ClueRooms.xlsx
+++ b/ClueRooms.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="2" documentId="11_7AB87FF4D80846A596E1D3CDB2CD715CF38999F4" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{86BFF185-3CE8-4527-8B40-0B5823156F71}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -130,7 +130,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -588,16 +588,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W37"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W20" sqref="F20:W20"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U12" sqref="U12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.6328125" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>3</v>
       </c>
@@ -668,7 +668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -739,7 +739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -810,7 +810,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -881,7 +881,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -952,7 +952,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>3</v>
       </c>
@@ -1094,7 +1094,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>1</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
@@ -1307,7 +1307,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
@@ -1378,7 +1378,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:23">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
@@ -1449,7 +1449,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:23">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>5</v>
       </c>
@@ -1520,7 +1520,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:23">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>5</v>
       </c>
@@ -1591,7 +1591,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:23">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>5</v>
       </c>
@@ -1662,7 +1662,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:23">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
@@ -1733,7 +1733,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:23">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>1</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:23">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:23">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>9</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:23">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>9</v>
       </c>
@@ -2017,7 +2017,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:23">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>9</v>
       </c>
@@ -2088,7 +2088,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:23">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>9</v>
       </c>
@@ -2159,7 +2159,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:23">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
@@ -2230,7 +2230,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:23">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>9</v>
       </c>
@@ -2301,7 +2301,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:23">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>9</v>
       </c>
@@ -2372,7 +2372,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:23">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0</v>
       </c>
@@ -2440,53 +2440,53 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:23">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:23">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B29" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:23">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:23">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B31" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D31" s="6"/>
     </row>
-    <row r="32" spans="1:23">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B32" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="2:2">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="2:2">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="2:2">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="2:2">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="16" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="2:2">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" s="6" t="s">
         <v>30</v>
       </c>

</xml_diff>